<commit_message>
Experiments 1 and 2!
Total re-write of the two experiments to fix errors found in logic and process complete! Analysis still needing further completion
</commit_message>
<xml_diff>
--- a/Data/Images/Experiment1A/Stats.xlsx
+++ b/Data/Images/Experiment1A/Stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C14460702\Dissertation\Data\Images\Experiment1A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB58FF9-F47F-4AFD-9F30-C88FD9640342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7F2B7B-223C-49EE-AE79-BB0721404C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11460" yWindow="1875" windowWidth="15375" windowHeight="7875" xr2:uid="{9CC51506-D779-46B0-8C16-FE34EA06A236}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9CC51506-D779-46B0-8C16-FE34EA06A236}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9DD5DD9-A914-4168-A54F-9886352F1DED}">
   <dimension ref="A4:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,10 +659,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="15">
-        <v>8.8079060000000001E-2</v>
+        <v>0.20432649999999999</v>
       </c>
       <c r="D7" s="16">
-        <v>1.200405E-2</v>
+        <v>2.421831E-2</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>0</v>
@@ -694,10 +694,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="15">
-        <v>8.8207820000000006E-2</v>
+        <v>0.2073287</v>
       </c>
       <c r="D8" s="16">
-        <v>1.2113799999999999E-2</v>
+        <v>2.544927E-2</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>1</v>
@@ -729,10 +729,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="19">
-        <v>9.212294E-2</v>
+        <v>0.19822629999999999</v>
       </c>
       <c r="D9" s="20">
-        <v>1.217125E-2</v>
+        <v>2.5111959999999999E-2</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>2</v>

</xml_diff>